<commit_message>
EPBDS-11247 enable property type validation for Action column if expression is empty
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DatatypeArray.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DatatypeArray.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D6A018-CD21-448B-BBC4-6A264DB84BA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17115" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case1" sheetId="10" r:id="rId1"/>
@@ -111,9 +117,6 @@
     <t>intValue</t>
   </si>
   <si>
-    <t>String return</t>
-  </si>
-  <si>
     <t>Return</t>
   </si>
   <si>
@@ -498,11 +501,14 @@
   <si>
     <t>Test intIndex</t>
   </si>
+  <si>
+    <t>String ret</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1152,20 +1158,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1192,6 +1184,9 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1212,6 +1207,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1244,18 +1250,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Обычный 2" xfId="4"/>
-    <cellStyle name="Обычный 3" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Обычный 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1406,9 +1415,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1446,9 +1455,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,9 +1490,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1516,9 +1542,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1691,11 +1734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,10 +1753,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -1740,10 +1783,10 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="43"/>
+      <c r="D7" s="37"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -1752,12 +1795,12 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="56"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1808,14 +1851,14 @@
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>30</v>
+      <c r="C12" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>29</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>14</v>
@@ -1831,40 +1874,40 @@
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="39" t="s">
-        <v>31</v>
+      <c r="C13" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="15">
         <v>40415</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="39" t="s">
-        <v>31</v>
+      <c r="C14" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="35"/>
+      <c r="K14" s="54"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="39" t="s">
-        <v>31</v>
+      <c r="C15" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>0</v>
@@ -1874,14 +1917,14 @@
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="39" t="s">
-        <v>31</v>
+      <c r="C16" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
@@ -1889,14 +1932,14 @@
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="39" t="s">
-        <v>31</v>
+      <c r="C17" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>11</v>
@@ -1906,11 +1949,11 @@
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="39" t="s">
-        <v>31</v>
+      <c r="C18" s="57" t="s">
+        <v>30</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="14">
         <v>40415.717464340276</v>
@@ -1924,7 +1967,7 @@
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1</v>
@@ -1942,16 +1985,16 @@
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E21" s="12"/>
     </row>
@@ -1960,7 +2003,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="12"/>
     </row>
@@ -1969,112 +2012,117 @@
         <v>21</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="12"/>
     </row>
     <row r="26" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>29</v>
+      <c r="C27" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>42</v>
+      <c r="C28" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="E28" s="13">
         <v>40415</v>
       </c>
       <c r="J28" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="38"/>
+      <c r="D29" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="44"/>
-      <c r="D29" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="44"/>
       <c r="E30" s="6" t="s">
         <v>24</v>
       </c>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="3:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="52"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="54" t="s">
+      <c r="D32" s="50"/>
+      <c r="E32" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="55"/>
-      <c r="E32" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="53"/>
-      <c r="E33" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="50" t="s">
+      <c r="D34" s="46"/>
+      <c r="E34" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="45" t="s">
+      <c r="D35" s="40"/>
+      <c r="E35" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="45" t="s">
+      <c r="D36" s="40"/>
+      <c r="E36" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="11" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="D29"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:C18"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C28:C29"/>
@@ -2087,11 +2135,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="D29"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2099,7 +2142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2117,15 +2160,15 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="58"/>
     </row>
@@ -2139,23 +2182,23 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E6" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -2165,26 +2208,26 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E13" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="58"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -2192,12 +2235,12 @@
         <v>10</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="60"/>
       <c r="F21" s="60"/>
@@ -2207,10 +2250,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
@@ -2222,10 +2265,10 @@
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="3">
         <v>12</v>
@@ -2233,10 +2276,10 @@
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="3">
         <v>23</v>
@@ -2244,7 +2287,7 @@
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E27" s="59"/>
       <c r="F27" s="59"/>
@@ -2258,17 +2301,17 @@
         <v>22</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="17"/>
     </row>
@@ -2277,24 +2320,24 @@
         <v>11</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G31" s="16">
         <v>23</v>
@@ -2302,13 +2345,13 @@
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="16">
         <v>22</v>
@@ -2326,7 +2369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2341,11 +2384,11 @@
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="58"/>
       <c r="F5" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" s="58"/>
     </row>
@@ -2354,13 +2397,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -2374,7 +2417,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -2382,95 +2425,95 @@
         <v>10</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="F10" s="59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G10" s="59"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="16"/>
       <c r="F12" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="16">
         <v>12</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="16">
         <v>23</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
@@ -2480,12 +2523,12 @@
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2500,7 +2543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2516,16 +2559,16 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="61"/>
       <c r="F6" s="62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" s="63"/>
       <c r="H6" s="63"/>
@@ -2539,28 +2582,28 @@
         <v>25</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="I7" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="24" t="s">
-        <v>87</v>
-      </c>
       <c r="J7" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="L7" s="24" t="s">
         <v>90</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
@@ -2568,10 +2611,10 @@
         <v>25</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -2585,28 +2628,28 @@
         <v>25</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="H9" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="I9" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="J9" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="K9" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="L9" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="L9" s="26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -2614,16 +2657,16 @@
         <v>10</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="H10" s="27" t="s">
         <v>103</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>104</v>
       </c>
       <c r="I10" s="27">
         <v>2000</v>
@@ -2640,19 +2683,19 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>89</v>
-      </c>
       <c r="F11" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="H11" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="I11" s="27">
         <v>1999</v>
@@ -2669,13 +2712,13 @@
     </row>
     <row r="12" spans="2:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="25.5" x14ac:dyDescent="0.25">
@@ -2683,42 +2726,42 @@
         <v>10</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="67"/>
       <c r="F16" s="64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="64"/>
       <c r="H16" s="65"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N17" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -2726,15 +2769,15 @@
         <v>25</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H18" s="25"/>
       <c r="N18" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -2742,18 +2785,18 @@
         <v>11</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F20" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="29">
         <v>3</v>
@@ -2761,10 +2804,10 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="29">
         <v>5</v>
@@ -2772,7 +2815,7 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N22" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -2782,7 +2825,7 @@
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N24" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -2804,7 +2847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B5:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2820,11 +2863,11 @@
   <sheetData>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="61"/>
       <c r="F5" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G5" s="63"/>
       <c r="H5" s="63"/>
@@ -2833,39 +2876,39 @@
       <c r="K5" s="63"/>
       <c r="L5" s="63"/>
       <c r="O5" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G6" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="I6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>87</v>
-      </c>
       <c r="J6" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="L6" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="O6" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -2873,10 +2916,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
@@ -2890,28 +2933,28 @@
         <v>25</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="I8" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="J8" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="L8" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -2919,16 +2962,16 @@
         <v>10</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="27">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>103</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>104</v>
       </c>
       <c r="I9" s="27">
         <v>2000</v>
@@ -2945,19 +2988,19 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>89</v>
       </c>
       <c r="F10" s="27">
         <v>8</v>
       </c>
       <c r="G10" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="I10" s="27">
         <v>1999</v>
@@ -2972,18 +3015,18 @@
         <v>8000</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2991,30 +3034,30 @@
         <v>10</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="67"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -3022,7 +3065,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3036,7 +3079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B5:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3051,11 +3094,11 @@
   <sheetData>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="61"/>
       <c r="F5" s="62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="63"/>
       <c r="H5" s="63"/>
@@ -3064,7 +3107,7 @@
       <c r="K5" s="63"/>
       <c r="L5" s="63"/>
       <c r="P5" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
@@ -3072,31 +3115,31 @@
         <v>10</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G6" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="I6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>87</v>
-      </c>
       <c r="J6" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="L6" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="P6" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -3104,10 +3147,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
@@ -3121,28 +3164,28 @@
         <v>25</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="I8" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="J8" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="L8" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -3150,16 +3193,16 @@
         <v>10</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="27">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>103</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>104</v>
       </c>
       <c r="I9" s="27">
         <v>2000</v>
@@ -3174,24 +3217,24 @@
         <v>12000</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>89</v>
       </c>
       <c r="F10" s="27">
         <v>8</v>
       </c>
       <c r="G10" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="I10" s="27">
         <v>1999</v>
@@ -3206,18 +3249,18 @@
         <v>8000</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -3225,25 +3268,25 @@
         <v>10</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="67"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -3251,7 +3294,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>